<commit_message>
shop all page more scenarios
</commit_message>
<xml_diff>
--- a/ecommerse_java_automation/project_documents.xlsx
+++ b/ecommerse_java_automation/project_documents.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D6862E-80FC-4039-B8E5-65BCB544FD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA52579-5457-4A3D-884B-3665DD7F2F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Homepage" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Emails" sheetId="8" r:id="rId8"/>
     <sheet name="Dashboardpage" sheetId="9" r:id="rId9"/>
     <sheet name="Cartpage" sheetId="10" r:id="rId10"/>
+    <sheet name="SingleProductPage" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="507">
   <si>
     <t>Pagename</t>
   </si>
@@ -1145,9 +1146,6 @@
     <t>Shop | ECODERS</t>
   </si>
   <si>
-    <t xml:space="preserve">a[href='/shop'],   </t>
-  </si>
-  <si>
     <t>//form//input[@type='text'],  //form[contains(@class,'max-w-2xl')]/input</t>
   </si>
   <si>
@@ -1780,9 +1778,6 @@
     <t xml:space="preserve">this is for the parent having heading., 13 items text, 3 views icons. </t>
   </si>
   <si>
-    <t>.flex.items-center.justify-between.mb-6&gt;h1</t>
-  </si>
-  <si>
     <t>our product heading</t>
   </si>
   <si>
@@ -1798,9 +1793,6 @@
     <t>//div[@class='flex items-center gap-2']/span</t>
   </si>
   <si>
-    <t>div.flex.items-center.gap-2&gt;span.text-sm.text-gray-500</t>
-  </si>
-  <si>
     <t>parent division having the 3 view icons</t>
   </si>
   <si>
@@ -2237,13 +2229,49 @@
   </si>
   <si>
     <t>Checkout navigation button</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">a[href='/shop']   a[target='_self']        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>a.linkText</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">.flex.items-center.justify-between.mb-6&gt;h1             </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">div.flex.items-center.gap-2&gt;span.text-sm.text-gray-500              .flex-grow.container.py-6&gt;div&gt;div:last-child&gt;div&gt;h1            </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   h1[class='text-3xl font-extrabold text-gray-800']</t>
+    </r>
+  </si>
+  <si>
+    <t>Single-Product | ECODERS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2308,6 +2336,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2326,10 +2368,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2374,8 +2417,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2715,7 +2760,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3178,7 +3223,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B1" t="s">
         <v>217</v>
@@ -3189,10 +3234,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C2" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3203,279 +3248,321 @@
         <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D5" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>429</v>
+      </c>
+      <c r="B6" t="s">
+        <v>430</v>
+      </c>
+      <c r="C6" t="s">
+        <v>431</v>
+      </c>
+      <c r="D6" t="s">
         <v>432</v>
-      </c>
-      <c r="B6" t="s">
-        <v>433</v>
-      </c>
-      <c r="C6" t="s">
-        <v>434</v>
-      </c>
-      <c r="D6" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>433</v>
+      </c>
+      <c r="B7" t="s">
+        <v>434</v>
+      </c>
+      <c r="C7" t="s">
+        <v>435</v>
+      </c>
+      <c r="D7" t="s">
         <v>436</v>
-      </c>
-      <c r="B7" t="s">
-        <v>437</v>
-      </c>
-      <c r="C7" t="s">
-        <v>438</v>
-      </c>
-      <c r="D7" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>437</v>
+      </c>
+      <c r="B8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C8" t="s">
+        <v>439</v>
+      </c>
+      <c r="D8" t="s">
         <v>440</v>
-      </c>
-      <c r="B8" t="s">
-        <v>441</v>
-      </c>
-      <c r="C8" t="s">
-        <v>442</v>
-      </c>
-      <c r="D8" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>441</v>
+      </c>
+      <c r="B9" t="s">
+        <v>442</v>
+      </c>
+      <c r="C9" t="s">
+        <v>443</v>
+      </c>
+      <c r="D9" t="s">
         <v>444</v>
-      </c>
-      <c r="B9" t="s">
-        <v>445</v>
-      </c>
-      <c r="C9" t="s">
-        <v>446</v>
-      </c>
-      <c r="D9" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>445</v>
+      </c>
+      <c r="B10" t="s">
+        <v>446</v>
+      </c>
+      <c r="C10" t="s">
+        <v>447</v>
+      </c>
+      <c r="D10" t="s">
         <v>448</v>
-      </c>
-      <c r="B10" t="s">
-        <v>449</v>
-      </c>
-      <c r="C10" t="s">
-        <v>450</v>
-      </c>
-      <c r="D10" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>449</v>
+      </c>
+      <c r="B11" t="s">
+        <v>450</v>
+      </c>
+      <c r="C11" t="s">
+        <v>451</v>
+      </c>
+      <c r="D11" t="s">
         <v>452</v>
-      </c>
-      <c r="B11" t="s">
-        <v>453</v>
-      </c>
-      <c r="C11" t="s">
-        <v>454</v>
-      </c>
-      <c r="D11" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>453</v>
+      </c>
+      <c r="B12" t="s">
+        <v>454</v>
+      </c>
+      <c r="C12" t="s">
+        <v>455</v>
+      </c>
+      <c r="D12" t="s">
         <v>456</v>
-      </c>
-      <c r="B12" t="s">
-        <v>457</v>
-      </c>
-      <c r="C12" t="s">
-        <v>458</v>
-      </c>
-      <c r="D12" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B13" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C13" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D13" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>460</v>
+      </c>
+      <c r="B14" t="s">
+        <v>461</v>
+      </c>
+      <c r="C14" t="s">
+        <v>462</v>
+      </c>
+      <c r="D14" t="s">
         <v>463</v>
-      </c>
-      <c r="B14" t="s">
-        <v>464</v>
-      </c>
-      <c r="C14" t="s">
-        <v>465</v>
-      </c>
-      <c r="D14" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>464</v>
+      </c>
+      <c r="B15" t="s">
+        <v>465</v>
+      </c>
+      <c r="C15" t="s">
+        <v>466</v>
+      </c>
+      <c r="D15" t="s">
         <v>467</v>
-      </c>
-      <c r="B15" t="s">
-        <v>468</v>
-      </c>
-      <c r="C15" t="s">
-        <v>469</v>
-      </c>
-      <c r="D15" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>468</v>
+      </c>
+      <c r="B16" t="s">
+        <v>469</v>
+      </c>
+      <c r="C16" t="s">
+        <v>470</v>
+      </c>
+      <c r="D16" t="s">
         <v>471</v>
-      </c>
-      <c r="B16" t="s">
-        <v>472</v>
-      </c>
-      <c r="C16" t="s">
-        <v>473</v>
-      </c>
-      <c r="D16" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>472</v>
+      </c>
+      <c r="B17" t="s">
+        <v>473</v>
+      </c>
+      <c r="C17" t="s">
+        <v>474</v>
+      </c>
+      <c r="D17" t="s">
         <v>475</v>
-      </c>
-      <c r="B17" t="s">
-        <v>476</v>
-      </c>
-      <c r="C17" t="s">
-        <v>477</v>
-      </c>
-      <c r="D17" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
+        <v>476</v>
+      </c>
+      <c r="B18" t="s">
+        <v>477</v>
+      </c>
+      <c r="C18" t="s">
+        <v>478</v>
+      </c>
+      <c r="D18" t="s">
         <v>479</v>
-      </c>
-      <c r="B18" t="s">
-        <v>480</v>
-      </c>
-      <c r="C18" t="s">
-        <v>481</v>
-      </c>
-      <c r="D18" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
+        <v>480</v>
+      </c>
+      <c r="B19" t="s">
+        <v>481</v>
+      </c>
+      <c r="C19" t="s">
+        <v>482</v>
+      </c>
+      <c r="D19" t="s">
         <v>483</v>
-      </c>
-      <c r="B19" t="s">
-        <v>484</v>
-      </c>
-      <c r="C19" t="s">
-        <v>485</v>
-      </c>
-      <c r="D19" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
+        <v>484</v>
+      </c>
+      <c r="B20" t="s">
+        <v>485</v>
+      </c>
+      <c r="C20" t="s">
+        <v>486</v>
+      </c>
+      <c r="D20" t="s">
         <v>487</v>
-      </c>
-      <c r="B20" t="s">
-        <v>488</v>
-      </c>
-      <c r="C20" t="s">
-        <v>489</v>
-      </c>
-      <c r="D20" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>488</v>
+      </c>
+      <c r="B21" t="s">
+        <v>489</v>
+      </c>
+      <c r="C21" t="s">
+        <v>490</v>
+      </c>
+      <c r="D21" t="s">
         <v>491</v>
-      </c>
-      <c r="B21" t="s">
-        <v>492</v>
-      </c>
-      <c r="C21" t="s">
-        <v>493</v>
-      </c>
-      <c r="D21" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B22" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C22" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D22" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
+        <v>495</v>
+      </c>
+      <c r="B23" t="s">
+        <v>496</v>
+      </c>
+      <c r="C23" t="s">
+        <v>497</v>
+      </c>
+      <c r="D23" t="s">
         <v>498</v>
-      </c>
-      <c r="B23" t="s">
-        <v>499</v>
-      </c>
-      <c r="C23" t="s">
-        <v>500</v>
-      </c>
-      <c r="D23" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
+        <v>499</v>
+      </c>
+      <c r="B24" t="s">
+        <v>500</v>
+      </c>
+      <c r="C24" t="s">
+        <v>501</v>
+      </c>
+      <c r="D24" t="s">
         <v>502</v>
       </c>
-      <c r="B24" t="s">
-        <v>503</v>
-      </c>
-      <c r="C24" t="s">
-        <v>504</v>
-      </c>
-      <c r="D24" t="s">
-        <v>505</v>
-      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83786577-345C-4B47-B4F3-BF60F78E0C17}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{B8DB0B2B-55A5-457C-8C55-CAA99E84714D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3484,8 +3571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3543,7 +3630,7 @@
         <v>215</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>220</v>
+        <v>503</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>175</v>
@@ -3568,7 +3655,7 @@
         <v>131</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>132</v>
@@ -3638,7 +3725,7 @@
         <v>141</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="9" t="s">
@@ -3951,8 +4038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3978,332 +4065,335 @@
       <c r="B2" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="18" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B4" t="s">
         <v>344</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>345</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>346</v>
-      </c>
-      <c r="D4" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B5" t="s">
         <v>348</v>
-      </c>
-      <c r="B5" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" t="s">
+        <v>349</v>
+      </c>
+      <c r="D6" t="s">
         <v>351</v>
-      </c>
-      <c r="C6" t="s">
-        <v>350</v>
-      </c>
-      <c r="D6" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C7" t="s">
-        <v>353</v>
+        <v>504</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C9" t="s">
-        <v>359</v>
+        <v>505</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B11" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C11" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B12" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C12" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C13" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C14" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C16" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C17" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C18" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C20" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C21" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C22" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C23" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C24" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C25" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C26" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C27" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C29" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C30" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C31" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C34" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C36" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
+        <v>399</v>
+      </c>
+      <c r="C37" t="s">
         <v>402</v>
-      </c>
-      <c r="C37" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C38" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
+        <v>403</v>
+      </c>
+      <c r="C40" t="s">
         <v>406</v>
-      </c>
-      <c r="C40" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C41" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C45" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C46" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C47" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C48" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C49" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C50" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C53" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C54" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{661E5213-82CD-42E4-BF59-1BFBBEB0B5B7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4319,7 +4409,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B1" t="s">
         <v>217</v>
@@ -4330,10 +4420,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -4353,7 +4443,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B1" t="s">
         <v>217</v>
@@ -4364,10 +4454,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" t="s">
         <v>226</v>
-      </c>
-      <c r="C2" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -4387,12 +4477,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18">
       <c r="A1" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75">
       <c r="A2" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -4400,12 +4490,12 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -4413,12 +4503,12 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -4426,17 +4516,17 @@
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75">
       <c r="A12" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:1">
@@ -4444,12 +4534,12 @@
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:1">
@@ -4457,12 +4547,12 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -4470,12 +4560,12 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:1">
@@ -4483,7 +4573,7 @@
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -4491,12 +4581,12 @@
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:1">
@@ -4504,12 +4594,12 @@
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:1">
@@ -4517,12 +4607,12 @@
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="33" spans="1:1">
@@ -4530,7 +4620,7 @@
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:1">
@@ -4538,27 +4628,27 @@
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:1">
@@ -4566,12 +4656,12 @@
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:1">
@@ -4579,7 +4669,7 @@
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:1">
@@ -4587,12 +4677,12 @@
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15.75">
       <c r="A48" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -4600,12 +4690,12 @@
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="52" spans="1:1">
@@ -4613,37 +4703,37 @@
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" spans="1:1">
@@ -4651,22 +4741,22 @@
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15.75">
       <c r="A62" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="65" spans="1:1">
@@ -4674,12 +4764,12 @@
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="68" spans="1:1">
@@ -4687,12 +4777,12 @@
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="71" spans="1:1">
@@ -4700,12 +4790,12 @@
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="74" spans="1:1">
@@ -4713,22 +4803,22 @@
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="79" spans="1:1">
@@ -4736,27 +4826,27 @@
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="15.75">
       <c r="A83" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="85" spans="1:1">
@@ -4764,17 +4854,17 @@
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="89" spans="1:1">
@@ -4782,17 +4872,17 @@
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="93" spans="1:1">
@@ -4800,17 +4890,17 @@
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15.75">
       <c r="A96" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="97" spans="1:1">
@@ -4818,12 +4908,12 @@
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="100" spans="1:1">
@@ -4831,7 +4921,7 @@
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="102" spans="1:1">
@@ -4839,12 +4929,12 @@
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15.75">
       <c r="A104" s="16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="105" spans="1:1">
@@ -4852,12 +4942,12 @@
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="108" spans="1:1">
@@ -4865,27 +4955,27 @@
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15.75">
       <c r="A113" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="114" spans="1:1">
@@ -4893,12 +4983,12 @@
     </row>
     <row r="115" spans="1:1">
       <c r="A115" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="117" spans="1:1">
@@ -4906,12 +4996,12 @@
     </row>
     <row r="118" spans="1:1">
       <c r="A118" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="120" spans="1:1">
@@ -4919,22 +5009,22 @@
     </row>
     <row r="121" spans="1:1">
       <c r="A121" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -4955,127 +5045,127 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="150">
       <c r="A10" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -5107,10 +5197,10 @@
     </row>
     <row r="2" spans="2:3">
       <c r="B2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>